<commit_message>
update scripts for chapter11
</commit_message>
<xml_diff>
--- a/Chapter11/Data/testdata.xlsx
+++ b/Chapter11/Data/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason118/PycharmProjects/selenium4.0-automation/Chapter11/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01A55953-256C-1543-A8D8-AFE01D6AA6D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B74C5D-35CA-0E4C-95AB-34CD9EECF2A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15600" xr2:uid="{521DF255-0147-2F4C-808F-D5E8169A43C3}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15600" activeTab="1" xr2:uid="{521DF255-0147-2F4C-808F-D5E8169A43C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029" calcOnSave="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>岗位名称</t>
   </si>
@@ -49,6 +50,18 @@
   </si>
   <si>
     <t>PostCode0305022022</t>
+  </si>
+  <si>
+    <t>用户名</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -402,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A852D082-1AE5-6840-B151-BD901842036A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,4 +450,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DA5B10-D0E7-C84F-A9C7-0BC89BD06B2B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>